<commit_message>
feat: Cleaner File IO
</commit_message>
<xml_diff>
--- a/Documents/Terminologies.xlsx
+++ b/Documents/Terminologies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Jupiter Technologies\Jupiter-Engine\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74857803-649F-4E91-8868-0AF021A536CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A3F9C2-E760-4E54-A2B8-3771A2C9B11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-1485" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Use</t>
   </si>
@@ -94,6 +94,24 @@
   </si>
   <si>
     <t>End</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t>From, Load</t>
+  </si>
+  <si>
+    <t>To, Save</t>
+  </si>
+  <si>
+    <t>System serialization Read</t>
+  </si>
+  <si>
+    <t>System serialization Write</t>
   </si>
 </sst>
 </file>
@@ -411,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,6 +542,28 @@
         <v>22</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor: new conventions - Foo:        i.e String - FooUtils:   i.e StringUtils. Depend on String. Free functions that manipulate strings - FooHelpers: i.e StringHelpers. String depends on StringHelpers. Help internal String implementations
</commit_message>
<xml_diff>
--- a/Documents/Terminologies.xlsx
+++ b/Documents/Terminologies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Jupiter Technologies\Jupiter-Engine\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A3F9C2-E760-4E54-A2B8-3771A2C9B11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3C70A3-ED25-4F1A-A122-6C870EA3EA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,12 +90,6 @@
     <t>Clean</t>
   </si>
   <si>
-    <t>Begin</t>
-  </si>
-  <si>
-    <t>End</t>
-  </si>
-  <si>
     <t>Read</t>
   </si>
   <si>
@@ -112,14 +106,28 @@
   </si>
   <si>
     <t>System serialization Write</t>
+  </si>
+  <si>
+    <t>Not O(1) get information or data</t>
+  </si>
+  <si>
+    <t>LookUp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -147,8 +155,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +441,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,13 +452,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -473,8 +482,14 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
       <c r="B4" t="s">
         <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -532,39 +547,30 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-    </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
         <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>